<commit_message>
- Update circuit for IR barrier - Add testing TRX - Update components - Update position of components on Layout - Update BOM
</commit_message>
<xml_diff>
--- a/Connect Medical Boards/EFM1/Project Outputs for 105358-3BA001-01_EFM1/105358-3BA001-04_EFM1_BOM.xlsx
+++ b/Connect Medical Boards/EFM1/Project Outputs for 105358-3BA001-01_EFM1/105358-3BA001-04_EFM1_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="183">
   <si>
     <t>Designator</t>
   </si>
@@ -144,7 +144,22 @@
     <t>478-10324-1-ND</t>
   </si>
   <si>
-    <t>C15</t>
+    <t>C15, C16</t>
+  </si>
+  <si>
+    <t>0.1µF ±10% 10V X5R Ceramic Capacitor 0402</t>
+  </si>
+  <si>
+    <t>0.1µF-10V</t>
+  </si>
+  <si>
+    <t>CC0402KRX5R6BB104</t>
+  </si>
+  <si>
+    <t>311-1336-1-ND</t>
+  </si>
+  <si>
+    <t>C17</t>
   </si>
   <si>
     <t>1.2nF ±10% 10V U2J Ceramic Capacitor 0402</t>
@@ -351,7 +366,7 @@
     <t>YAG3452CT-ND</t>
   </si>
   <si>
-    <t>R5, R9, R10, R12</t>
+    <t>R5, R13, R14, R17</t>
   </si>
   <si>
     <t>RES SMD 10kOHM 1% 1/16W 0402</t>
@@ -381,7 +396,7 @@
     <t>311-5.6KJRCT-ND</t>
   </si>
   <si>
-    <t>R7</t>
+    <t>R7, R11, R12</t>
   </si>
   <si>
     <t>RES SMD 41.2kOHM 1% 1/16W 0402</t>
@@ -396,7 +411,13 @@
     <t>YAG3155CT-ND</t>
   </si>
   <si>
-    <t>R8</t>
+    <t>R8, R9, R18, R19</t>
+  </si>
+  <si>
+    <t>Do Not Place</t>
+  </si>
+  <si>
+    <t>R10</t>
   </si>
   <si>
     <t>RES SMD 390kOHM 1% 1/16W 0402</t>
@@ -411,7 +432,7 @@
     <t>YAG3143CT-ND</t>
   </si>
   <si>
-    <t>R11</t>
+    <t>R15</t>
   </si>
   <si>
     <t>RES SMD 100OHM 1% 1/16W 0402</t>
@@ -426,7 +447,7 @@
     <t>311-100LRCT-ND</t>
   </si>
   <si>
-    <t>R13</t>
+    <t>R16</t>
   </si>
   <si>
     <t>RES SMD 0.0OHM JUMPER 1/16W 0402</t>
@@ -896,7 +917,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1097,7 +1118,7 @@
         <v>43</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>44</v>
@@ -1109,7 +1130,7 @@
         <v>15</v>
       </c>
       <c r="H7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>16</v>
@@ -1126,16 +1147,16 @@
         <v>48</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>50</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="3">
         <v>1</v>
@@ -1178,22 +1199,22 @@
         <v>56</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H10" s="3">
         <v>1</v>
@@ -1204,25 +1225,25 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>63</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="H11" s="3">
         <v>1</v>
@@ -1251,7 +1272,7 @@
         <v>68</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="H12" s="3">
         <v>1</v>
@@ -1271,16 +1292,16 @@
         <v>71</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
@@ -1291,25 +1312,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -1329,16 +1350,16 @@
         <v>82</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H15" s="3">
         <v>1</v>
@@ -1358,16 +1379,16 @@
         <v>87</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="H16" s="3">
         <v>1</v>
@@ -1387,16 +1408,16 @@
         <v>92</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="H17" s="3">
         <v>1</v>
@@ -1407,16 +1428,16 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>97</v>
@@ -1425,33 +1446,33 @@
         <v>98</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H18" s="3">
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>15</v>
@@ -1460,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1486,10 +1507,10 @@
         <v>15</v>
       </c>
       <c r="H20" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1515,10 +1536,10 @@
         <v>15</v>
       </c>
       <c r="H21" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1544,10 +1565,10 @@
         <v>15</v>
       </c>
       <c r="H22" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1576,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1602,10 +1623,10 @@
         <v>15</v>
       </c>
       <c r="H24" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1616,45 +1637,45 @@
         <v>131</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>133</v>
+        <v>16</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H25" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>15</v>
@@ -1663,91 +1684,91 @@
         <v>1</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H27" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="G28" s="2" t="s">
-        <v>151</v>
+        <v>15</v>
       </c>
       <c r="H28" s="3">
         <v>1</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="G29" s="2" t="s">
-        <v>156</v>
+        <v>16</v>
       </c>
       <c r="H29" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>16</v>
@@ -1755,25 +1776,25 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="H30" s="3">
         <v>1</v>
@@ -1784,25 +1805,25 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="H31" s="3">
         <v>1</v>
@@ -1813,30 +1834,88 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="H32" s="3">
+        <v>1</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F32" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="E33" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="H32" s="3">
-        <v>1</v>
-      </c>
-      <c r="I32" s="2" t="s">
+      <c r="G33" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H33" s="3">
+        <v>1</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H34" s="3">
+        <v>1</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Add R20 to reduce current consumption to MOUNT_SWITCH signal in MCU - Allocate component - Update BOM
</commit_message>
<xml_diff>
--- a/Connect Medical Boards/EFM1/Project Outputs for 105358-3BA001-01_EFM1/105358-3BA001-04_EFM1_BOM.xlsx
+++ b/Connect Medical Boards/EFM1/Project Outputs for 105358-3BA001-01_EFM1/105358-3BA001-04_EFM1_BOM.xlsx
@@ -318,7 +318,7 @@
     <t>754-1436-1-ND</t>
   </si>
   <si>
-    <t>R1</t>
+    <t>R1, R20</t>
   </si>
   <si>
     <t>RES SMD 820kOHM 1% 1/16W 0402</t>
@@ -1478,7 +1478,7 @@
         <v>15</v>
       </c>
       <c r="H19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>104</v>

</xml_diff>